<commit_message>
update part 2 notebook
</commit_message>
<xml_diff>
--- a/From Excel to Python - Part 2/data/Monthly Sales Report.xlsx
+++ b/From Excel to Python - Part 2/data/Monthly Sales Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonasschroeder/OneDrive - MTP-Marketing zwischen Theorie und Praxis e. V/HOSD_Mentoring/HOSD repo/presentations/From Excel to Python - Part 2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B66AF2C-777F-CF40-B797-382604696BDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF272D3E-FCDA-8C49-AFC1-353B52B25AE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{C5E7E521-643D-CE43-84A9-BCF01C463588}"/>
   </bookViews>
@@ -599,7 +599,7 @@
                   <c:v>679</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>821</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -721,7 +721,7 @@
                   <c:v>5793</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5237</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -843,7 +843,7 @@
                   <c:v>3561</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5071</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -967,7 +967,7 @@
                   <c:v>256</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>190</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -1359,7 +1359,7 @@
                   <c:v>2199</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3161</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -1481,7 +1481,7 @@
                   <c:v>2899</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>481</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -1603,7 +1603,7 @@
                   <c:v>3169</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5282</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -1727,7 +1727,7 @@
                   <c:v>2022</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2395</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -2118,7 +2118,7 @@
                   <c:v>2199</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3161</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -2237,7 +2237,7 @@
                   <c:v>2899</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>481</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -2356,7 +2356,7 @@
                   <c:v>3169</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5282</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -2477,7 +2477,7 @@
                   <c:v>2022</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2395</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -4760,7 +4760,7 @@
   <dimension ref="B2:O34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W24" sqref="W24"/>
+      <selection activeCell="Q29" sqref="Q29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4900,7 +4900,7 @@
         <v>679</v>
       </c>
       <c r="I8" s="10">
-        <v>821</v>
+        <v>0</v>
       </c>
       <c r="J8" s="10">
         <v>0</v>
@@ -4919,7 +4919,7 @@
       </c>
       <c r="O8" s="10">
         <f t="shared" ref="O8:O11" si="0">SUM(C8:N8)</f>
-        <v>3337</v>
+        <v>2516</v>
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.2">
@@ -4945,7 +4945,7 @@
         <v>5793</v>
       </c>
       <c r="I9" s="10">
-        <v>5237</v>
+        <v>0</v>
       </c>
       <c r="J9" s="10">
         <v>0</v>
@@ -4964,7 +4964,7 @@
       </c>
       <c r="O9" s="10">
         <f t="shared" si="0"/>
-        <v>43821</v>
+        <v>38584</v>
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.2">
@@ -4990,7 +4990,7 @@
         <v>3561</v>
       </c>
       <c r="I10" s="10">
-        <v>5071</v>
+        <v>0</v>
       </c>
       <c r="J10" s="10">
         <v>0</v>
@@ -5009,7 +5009,7 @@
       </c>
       <c r="O10" s="10">
         <f t="shared" si="0"/>
-        <v>22279</v>
+        <v>17208</v>
       </c>
     </row>
     <row r="11" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -5035,7 +5035,7 @@
         <v>256</v>
       </c>
       <c r="I11" s="12">
-        <v>190</v>
+        <v>0</v>
       </c>
       <c r="J11" s="12">
         <v>0</v>
@@ -5054,7 +5054,7 @@
       </c>
       <c r="O11" s="12">
         <f t="shared" si="0"/>
-        <v>3034</v>
+        <v>2844</v>
       </c>
     </row>
     <row r="12" spans="2:15" ht="17" thickTop="1" x14ac:dyDescent="0.2">
@@ -5087,7 +5087,7 @@
       </c>
       <c r="I12" s="10">
         <f t="shared" ref="I12:J12" si="2">SUM(I8:I11)</f>
-        <v>11319</v>
+        <v>0</v>
       </c>
       <c r="J12" s="10">
         <f t="shared" si="2"/>
@@ -5111,7 +5111,7 @@
       </c>
       <c r="O12" s="10">
         <f>SUM(C12:N12)</f>
-        <v>72471</v>
+        <v>61152</v>
       </c>
     </row>
     <row r="29" spans="2:15" ht="26" x14ac:dyDescent="0.3">
@@ -5184,7 +5184,7 @@
         <v>2199</v>
       </c>
       <c r="I31" s="10">
-        <v>3161</v>
+        <v>0</v>
       </c>
       <c r="J31" s="10">
         <v>0</v>
@@ -5203,7 +5203,7 @@
       </c>
       <c r="O31" s="10">
         <f t="shared" ref="O31:O34" si="3">SUM(C31:N31)</f>
-        <v>14055</v>
+        <v>10894</v>
       </c>
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.2">
@@ -5229,7 +5229,7 @@
         <v>2899</v>
       </c>
       <c r="I32" s="10">
-        <v>481</v>
+        <v>0</v>
       </c>
       <c r="J32" s="10">
         <v>0</v>
@@ -5248,7 +5248,7 @@
       </c>
       <c r="O32" s="10">
         <f t="shared" si="3"/>
-        <v>15152</v>
+        <v>14671</v>
       </c>
     </row>
     <row r="33" spans="2:15" x14ac:dyDescent="0.2">
@@ -5274,7 +5274,7 @@
         <v>3169</v>
       </c>
       <c r="I33" s="10">
-        <v>5282</v>
+        <v>0</v>
       </c>
       <c r="J33" s="10">
         <v>0</v>
@@ -5293,7 +5293,7 @@
       </c>
       <c r="O33" s="10">
         <f t="shared" si="3"/>
-        <v>24190</v>
+        <v>18908</v>
       </c>
     </row>
     <row r="34" spans="2:15" x14ac:dyDescent="0.2">
@@ -5319,7 +5319,7 @@
         <v>2022</v>
       </c>
       <c r="I34" s="10">
-        <v>2395</v>
+        <v>0</v>
       </c>
       <c r="J34" s="10">
         <v>0</v>
@@ -5338,7 +5338,7 @@
       </c>
       <c r="O34" s="10">
         <f t="shared" si="3"/>
-        <v>19074</v>
+        <v>16679</v>
       </c>
     </row>
   </sheetData>

</xml_diff>